<commit_message>
updated canine breed xl files with stat bar query
</commit_message>
<xml_diff>
--- a/InputFiles/TC05_Canine_Filter_Breed-Beagle.xlsx
+++ b/InputFiles/TC05_Canine_Filter_Breed-Beagle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134F5100-7314-4F0B-ADBA-4FEBC0C34DD8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1B53C2-74A5-4246-9CBA-44CE333A41C7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -426,8 +426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>